<commit_message>
Started to work on the type-extensions, no karma specs have been ran yet
</commit_message>
<xml_diff>
--- a/Documents/Validators.xlsx
+++ b/Documents/Validators.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
@@ -20,7 +20,7 @@
     <author>Author</author>
   </authors>
   <commentList>
-    <comment ref="A16" authorId="0">
+    <comment ref="A16" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -49,7 +49,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="147" uniqueCount="92">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="147" uniqueCount="94">
   <si>
     <t>String</t>
   </si>
@@ -367,6 +367,12 @@
   </si>
   <si>
     <t>{} should not end with {}, but {} does</t>
+  </si>
+  <si>
+    <t>Y- Test</t>
+  </si>
+  <si>
+    <t>Y-Test</t>
   </si>
 </sst>
 </file>
@@ -512,6 +518,9 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
   </extLst>
 </styleSheet>
 </file>
@@ -559,7 +568,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -594,7 +603,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -805,8 +814,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J20" sqref="J20"/>
+    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
+      <selection activeCell="K15" sqref="K15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -857,16 +866,16 @@
         <v>3</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>13</v>
+        <v>92</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>13</v>
+        <v>92</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>13</v>
+        <v>92</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>13</v>
+        <v>92</v>
       </c>
       <c r="H2" t="s">
         <v>16</v>
@@ -886,16 +895,16 @@
         <v>44</v>
       </c>
       <c r="C3" s="5" t="s">
-        <v>13</v>
+        <v>92</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>13</v>
+        <v>92</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>13</v>
+        <v>92</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>13</v>
+        <v>93</v>
       </c>
       <c r="H3" t="s">
         <v>16</v>

</xml_diff>

<commit_message>
Implemented more methods, trying to fix Karma
</commit_message>
<xml_diff>
--- a/Documents/Validators.xlsx
+++ b/Documents/Validators.xlsx
@@ -49,7 +49,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="147" uniqueCount="94">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="147" uniqueCount="95">
   <si>
     <t>String</t>
   </si>
@@ -373,6 +373,9 @@
   </si>
   <si>
     <t>Y-Test</t>
+  </si>
+  <si>
+    <t>X - Test</t>
   </si>
 </sst>
 </file>
@@ -814,8 +817,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J20"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
-      <selection activeCell="K15" sqref="K15"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -921,16 +924,16 @@
         <v>5</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>13</v>
+        <v>92</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>13</v>
+        <v>94</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>13</v>
+        <v>92</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>13</v>
+        <v>93</v>
       </c>
       <c r="H4" t="s">
         <v>16</v>
@@ -947,16 +950,16 @@
         <v>46</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>13</v>
+        <v>92</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>13</v>
+        <v>92</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>13</v>
+        <v>92</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>13</v>
+        <v>93</v>
       </c>
       <c r="H5" t="s">
         <v>15</v>
@@ -976,7 +979,7 @@
         <v>34</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>13</v>
+        <v>92</v>
       </c>
       <c r="H6" t="s">
         <v>15</v>
@@ -996,7 +999,7 @@
         <v>35</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>13</v>
+        <v>92</v>
       </c>
       <c r="H7" t="s">
         <v>15</v>

</xml_diff>

<commit_message>
Minor document changes, put the validator.xlsx on google drive
</commit_message>
<xml_diff>
--- a/Documents/Validators.xlsx
+++ b/Documents/Validators.xlsx
@@ -49,7 +49,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="147" uniqueCount="95">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="147" uniqueCount="93">
   <si>
     <t>String</t>
   </si>
@@ -369,13 +369,7 @@
     <t>{} should not end with {}, but {} does</t>
   </si>
   <si>
-    <t>Y- Test</t>
-  </si>
-  <si>
     <t>Y-Test</t>
-  </si>
-  <si>
-    <t>X - Test</t>
   </si>
 </sst>
 </file>
@@ -817,8 +811,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J20"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="B2" sqref="A2:J20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -871,13 +865,13 @@
       <c r="C2" s="5" t="s">
         <v>92</v>
       </c>
-      <c r="D2" s="1" t="s">
-        <v>92</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>92</v>
-      </c>
-      <c r="F2" s="1" t="s">
+      <c r="D2" s="5" t="s">
+        <v>92</v>
+      </c>
+      <c r="E2" s="5" t="s">
+        <v>92</v>
+      </c>
+      <c r="F2" s="5" t="s">
         <v>92</v>
       </c>
       <c r="H2" t="s">
@@ -900,14 +894,14 @@
       <c r="C3" s="5" t="s">
         <v>92</v>
       </c>
-      <c r="D3" s="1" t="s">
-        <v>92</v>
-      </c>
-      <c r="E3" s="1" t="s">
-        <v>92</v>
-      </c>
-      <c r="F3" s="1" t="s">
-        <v>93</v>
+      <c r="D3" s="5" t="s">
+        <v>92</v>
+      </c>
+      <c r="E3" s="5" t="s">
+        <v>92</v>
+      </c>
+      <c r="F3" s="5" t="s">
+        <v>92</v>
       </c>
       <c r="H3" t="s">
         <v>16</v>
@@ -926,14 +920,14 @@
       <c r="C4" s="5" t="s">
         <v>92</v>
       </c>
-      <c r="D4" s="1" t="s">
-        <v>94</v>
-      </c>
-      <c r="E4" s="1" t="s">
-        <v>92</v>
-      </c>
-      <c r="F4" s="1" t="s">
-        <v>93</v>
+      <c r="D4" s="5" t="s">
+        <v>92</v>
+      </c>
+      <c r="E4" s="5" t="s">
+        <v>92</v>
+      </c>
+      <c r="F4" s="5" t="s">
+        <v>92</v>
       </c>
       <c r="H4" t="s">
         <v>16</v>
@@ -952,14 +946,14 @@
       <c r="C5" s="5" t="s">
         <v>92</v>
       </c>
-      <c r="D5" s="1" t="s">
-        <v>92</v>
-      </c>
-      <c r="E5" s="1" t="s">
-        <v>92</v>
-      </c>
-      <c r="F5" s="1" t="s">
-        <v>93</v>
+      <c r="D5" s="5" t="s">
+        <v>92</v>
+      </c>
+      <c r="E5" s="5" t="s">
+        <v>92</v>
+      </c>
+      <c r="F5" s="5" t="s">
+        <v>92</v>
       </c>
       <c r="H5" t="s">
         <v>15</v>
@@ -1019,7 +1013,7 @@
         <v>36</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>13</v>
+        <v>92</v>
       </c>
       <c r="H8" t="s">
         <v>15</v>
@@ -1039,7 +1033,7 @@
         <v>37</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>13</v>
+        <v>92</v>
       </c>
       <c r="H9" t="s">
         <v>15</v>

</xml_diff>

<commit_message>
Added some tasks to Grunt.js
</commit_message>
<xml_diff>
--- a/Documents/Validators.xlsx
+++ b/Documents/Validators.xlsx
@@ -811,8 +811,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J20"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="B2" sqref="A2:J20"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Updated Karma Specs, tests written
</commit_message>
<xml_diff>
--- a/Documents/Validators.xlsx
+++ b/Documents/Validators.xlsx
@@ -812,7 +812,7 @@
   <dimension ref="A1:J20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F12" sqref="F12"/>
+      <selection activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1084,7 +1084,7 @@
         <v>92</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>13</v>
+        <v>92</v>
       </c>
       <c r="H12" t="s">
         <v>15</v>
@@ -1104,10 +1104,10 @@
         <v>39</v>
       </c>
       <c r="C13" s="5" t="s">
-        <v>13</v>
+        <v>92</v>
       </c>
       <c r="F13" s="1" t="s">
-        <v>13</v>
+        <v>92</v>
       </c>
       <c r="H13" t="s">
         <v>15</v>
@@ -1127,7 +1127,7 @@
         <v>40</v>
       </c>
       <c r="C14" s="5" t="s">
-        <v>13</v>
+        <v>92</v>
       </c>
       <c r="F14" s="1" t="s">
         <v>13</v>

</xml_diff>

<commit_message>
More specs have been written
</commit_message>
<xml_diff>
--- a/Documents/Validators.xlsx
+++ b/Documents/Validators.xlsx
@@ -49,7 +49,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="147" uniqueCount="93">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="148" uniqueCount="93">
   <si>
     <t>String</t>
   </si>
@@ -812,7 +812,7 @@
   <dimension ref="A1:J20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F14" sqref="F14"/>
+      <selection activeCell="I18" sqref="I18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1130,7 +1130,7 @@
         <v>92</v>
       </c>
       <c r="F14" s="1" t="s">
-        <v>13</v>
+        <v>92</v>
       </c>
       <c r="H14" t="s">
         <v>15</v>
@@ -1150,10 +1150,10 @@
         <v>41</v>
       </c>
       <c r="C15" s="5" t="s">
-        <v>13</v>
+        <v>92</v>
       </c>
       <c r="F15" s="1" t="s">
-        <v>13</v>
+        <v>92</v>
       </c>
       <c r="H15" t="s">
         <v>15</v>
@@ -1173,7 +1173,10 @@
         <v>43</v>
       </c>
       <c r="C16" s="5" t="s">
-        <v>13</v>
+        <v>92</v>
+      </c>
+      <c r="F16" s="1" t="s">
+        <v>92</v>
       </c>
       <c r="H16" t="s">
         <v>15</v>
@@ -1193,10 +1196,10 @@
         <v>48</v>
       </c>
       <c r="C17" s="5" t="s">
-        <v>13</v>
+        <v>92</v>
       </c>
       <c r="F17" s="1" t="s">
-        <v>13</v>
+        <v>92</v>
       </c>
       <c r="H17" t="s">
         <v>15</v>

</xml_diff>

<commit_message>
Minor Adjustments to the Contract.ts, added some more specs and documentation has been written, editing currently in progress
</commit_message>
<xml_diff>
--- a/Documents/Validators.xlsx
+++ b/Documents/Validators.xlsx
@@ -49,7 +49,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="148" uniqueCount="93">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="148" uniqueCount="92">
   <si>
     <t>String</t>
   </si>
@@ -88,9 +88,6 @@
   </si>
   <si>
     <t>IsFalse</t>
-  </si>
-  <si>
-    <t>X</t>
   </si>
   <si>
     <t>Thrown Error</t>
@@ -828,10 +825,10 @@
   <sheetData>
     <row r="1" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="B1" s="2" t="s">
         <v>31</v>
-      </c>
-      <c r="B1" s="2" t="s">
-        <v>32</v>
       </c>
       <c r="C1" s="4" t="s">
         <v>0</v>
@@ -846,42 +843,42 @@
         <v>8</v>
       </c>
       <c r="H1" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="I1" s="8" t="s">
+        <v>54</v>
+      </c>
+      <c r="J1" s="8" t="s">
         <v>55</v>
-      </c>
-      <c r="J1" s="8" t="s">
-        <v>56</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B2" t="s">
         <v>3</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="D2" s="5" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="E2" s="5" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="F2" s="5" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="H2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="I2" s="9" t="s">
+        <v>56</v>
+      </c>
+      <c r="J2" s="9" t="s">
         <v>57</v>
-      </c>
-      <c r="J2" s="9" t="s">
-        <v>58</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
@@ -889,28 +886,28 @@
         <v>4</v>
       </c>
       <c r="B3" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C3" s="5" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="D3" s="5" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="E3" s="5" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="F3" s="5" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="H3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="I3" s="9" t="s">
+        <v>58</v>
+      </c>
+      <c r="J3" s="9" t="s">
         <v>59</v>
-      </c>
-      <c r="J3" s="9" t="s">
-        <v>60</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
@@ -918,51 +915,51 @@
         <v>5</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="D4" s="5" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="E4" s="5" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="F4" s="5" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="H4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="J4" s="9" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
+        <v>44</v>
+      </c>
+      <c r="B5" t="s">
         <v>45</v>
       </c>
-      <c r="B5" t="s">
-        <v>46</v>
-      </c>
       <c r="C5" s="5" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="D5" s="5" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="E5" s="5" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="F5" s="5" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="H5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="I5" s="9" t="s">
+        <v>61</v>
+      </c>
+      <c r="J5" s="9" t="s">
         <v>62</v>
-      </c>
-      <c r="J5" s="9" t="s">
-        <v>63</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
@@ -970,19 +967,19 @@
         <v>6</v>
       </c>
       <c r="B6" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="H6" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="I6" s="9" t="s">
+        <v>63</v>
+      </c>
+      <c r="J6" s="9" t="s">
         <v>64</v>
-      </c>
-      <c r="J6" s="9" t="s">
-        <v>65</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
@@ -990,19 +987,19 @@
         <v>7</v>
       </c>
       <c r="B7" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="H7" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="I7" s="9" t="s">
+        <v>65</v>
+      </c>
+      <c r="J7" s="9" t="s">
         <v>66</v>
-      </c>
-      <c r="J7" s="9" t="s">
-        <v>67</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
@@ -1010,19 +1007,19 @@
         <v>9</v>
       </c>
       <c r="B8" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="H8" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="I8" s="9" t="s">
+        <v>67</v>
+      </c>
+      <c r="J8" s="9" t="s">
         <v>68</v>
-      </c>
-      <c r="J8" s="9" t="s">
-        <v>69</v>
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
@@ -1030,19 +1027,19 @@
         <v>10</v>
       </c>
       <c r="B9" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="H9" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="I9" s="9" t="s">
+        <v>69</v>
+      </c>
+      <c r="J9" s="9" t="s">
         <v>70</v>
-      </c>
-      <c r="J9" s="9" t="s">
-        <v>71</v>
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
@@ -1050,13 +1047,13 @@
         <v>11</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="H10" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="I10" s="9" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
@@ -1064,214 +1061,214 @@
         <v>12</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="H11" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="I11" s="9" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B12" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C12" s="5" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="H12" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="I12" s="9" t="s">
+        <v>73</v>
+      </c>
+      <c r="J12" s="9" t="s">
         <v>74</v>
-      </c>
-      <c r="J12" s="9" t="s">
-        <v>75</v>
       </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B13" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C13" s="5" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="F13" s="1" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="H13" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="I13" s="9" t="s">
+        <v>75</v>
+      </c>
+      <c r="J13" s="9" t="s">
         <v>76</v>
-      </c>
-      <c r="J13" s="9" t="s">
-        <v>77</v>
       </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B14" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C14" s="5" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="F14" s="1" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="H14" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="I14" s="9" t="s">
+        <v>77</v>
+      </c>
+      <c r="J14" s="9" t="s">
         <v>78</v>
-      </c>
-      <c r="J14" s="9" t="s">
-        <v>79</v>
       </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B15" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C15" s="5" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="F15" s="1" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="H15" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="I15" s="9" t="s">
+        <v>79</v>
+      </c>
+      <c r="J15" s="9" t="s">
         <v>80</v>
-      </c>
-      <c r="J15" s="9" t="s">
-        <v>81</v>
       </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
+        <v>41</v>
+      </c>
+      <c r="B16" t="s">
         <v>42</v>
       </c>
-      <c r="B16" t="s">
-        <v>43</v>
-      </c>
       <c r="C16" s="5" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="F16" s="1" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="H16" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="I16" s="9" t="s">
+        <v>81</v>
+      </c>
+      <c r="J16" s="9" t="s">
         <v>82</v>
-      </c>
-      <c r="J16" s="9" t="s">
-        <v>83</v>
       </c>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
+        <v>46</v>
+      </c>
+      <c r="B17" t="s">
         <v>47</v>
       </c>
-      <c r="B17" t="s">
-        <v>48</v>
-      </c>
       <c r="C17" s="5" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="F17" s="1" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="H17" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="I17" s="9" t="s">
+        <v>83</v>
+      </c>
+      <c r="J17" s="9" t="s">
         <v>84</v>
-      </c>
-      <c r="J17" s="9" t="s">
-        <v>85</v>
       </c>
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
+        <v>48</v>
+      </c>
+      <c r="B18" t="s">
         <v>49</v>
       </c>
-      <c r="B18" t="s">
-        <v>50</v>
-      </c>
       <c r="C18" s="5" t="s">
-        <v>13</v>
+        <v>91</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>13</v>
+        <v>91</v>
       </c>
       <c r="H18" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="I18" s="9" t="s">
+        <v>85</v>
+      </c>
+      <c r="J18" s="9" t="s">
         <v>86</v>
-      </c>
-      <c r="J18" s="9" t="s">
-        <v>87</v>
       </c>
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
+        <v>50</v>
+      </c>
+      <c r="B19" t="s">
         <v>51</v>
       </c>
-      <c r="B19" t="s">
-        <v>52</v>
-      </c>
       <c r="C19" s="5" t="s">
-        <v>13</v>
+        <v>91</v>
       </c>
       <c r="H19" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="I19" s="9" t="s">
+        <v>87</v>
+      </c>
+      <c r="J19" s="9" t="s">
         <v>88</v>
-      </c>
-      <c r="J19" s="9" t="s">
-        <v>89</v>
       </c>
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
+        <v>52</v>
+      </c>
+      <c r="B20" t="s">
         <v>53</v>
       </c>
-      <c r="B20" t="s">
-        <v>54</v>
-      </c>
       <c r="C20" s="5" t="s">
-        <v>13</v>
+        <v>91</v>
       </c>
       <c r="H20" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="I20" s="9" t="s">
+        <v>89</v>
+      </c>
+      <c r="J20" s="9" t="s">
         <v>90</v>
-      </c>
-      <c r="J20" s="9" t="s">
-        <v>91</v>
       </c>
     </row>
   </sheetData>
@@ -1297,50 +1294,50 @@
   <sheetData>
     <row r="1" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="B1" s="6" t="s">
         <v>17</v>
-      </c>
-      <c r="B1" s="6" t="s">
-        <v>18</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B3" s="6" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="45" x14ac:dyDescent="0.25">
       <c r="A4" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="B4" s="7" t="s">
         <v>21</v>
-      </c>
-      <c r="B4" s="7" t="s">
-        <v>22</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="B5" s="6" t="s">
         <v>23</v>
-      </c>
-      <c r="B5" s="6" t="s">
-        <v>24</v>
       </c>
     </row>
     <row r="6" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A6" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="B6" s="6" t="s">
         <v>25</v>
-      </c>
-      <c r="B6" s="6" t="s">
-        <v>26</v>
       </c>
     </row>
   </sheetData>

</xml_diff>